<commit_message>
[ADD] ajout du nouveaux template
</commit_message>
<xml_diff>
--- a/admin/questions_files/template/Template_Questions.xlsx
+++ b/admin/questions_files/template/Template_Questions.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41630180-EB51-4294-9835-4F43EC660F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="3" r:id="rId1"/>
     <sheet name="Textes" sheetId="2" r:id="rId2"/>
+    <sheet name="Introduction" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Intitulé de la question (ex : quelle est votre adresse mail ?)</t>
   </si>
   <si>
+    <t>Créer autant de colonnes que de réponses possible (avec leurs noms). Attention si vous avez une réponse autre ne l'ajouté pas en temps que colonne.</t>
+  </si>
+  <si>
     <t>Bouton de validation</t>
   </si>
   <si>
@@ -44,19 +50,34 @@
     <t>Démarrer</t>
   </si>
   <si>
+    <t>Type de réponse attendu : "text", "radio" (choix unique), "checkbox" (choix multiple). Si vous souhaitez indiquer une réponse autre à votre réponse à choix multiple ou unique, indiquer : "checkbox, text" ou "radio, text"</t>
+  </si>
+  <si>
     <t>Combinatoire ( 0 si pas  de réponse particulière est attendu, "2, F" si la réponse attendu à la question de la 2ème ligne est la réponse de la colonne F)</t>
   </si>
   <si>
-    <t>Type de réponse attendu : "text", "radio" (choix unique), "checkbox" (choix multiple). Si vous souhaitez indiquer un champ "Autre" à votre réponse à choix multiple ou unique, indiquer : "checkbox, text" ou "radio, text"</t>
-  </si>
-  <si>
-    <t>Créer autant de colonnes que de réponses possible (avec leurs noms). Attention si vous avez un champ "Autre" ne l'ajoutez pas en temps que colonne.</t>
+    <t>RGPD</t>
+  </si>
+  <si>
+    <t>Ce questionnaire effectue une récolte de vos données personnelles (caractéristiques physiques, goûts, coordonnées notamment) ainsi que de données sur la manière dont vous le remplissez (vitesse, hésitations, changements, etc.). Ces données seront utilisées à des fins de recherches dans le cadre des travaux de Mme Jessica Pidoux. Pour toute demande concernant la gestion des données personnelles, envoyer un mail à l'adresse 'jessica.pidoux@epfl.ch'</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Le questionnaire est divisé en plusieurs phases : une phase de questions de départ sur votre sexe et votre orientation sexuelle, plusieurs phases de classement, une phase de questions supplémentaires à la fin. Lors des phases de classement, vous devrez déplacer avec la souris des descriptions de caractéristiques vers une échelle d'importance.</t>
+  </si>
+  <si>
+    <t>Validation du RGPD</t>
+  </si>
+  <si>
+    <t>Cochez la case si vous acceptez les conditions ci-dessus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -110,6 +131,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -209,6 +233,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -244,6 +285,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,16 +477,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="38.42578125" defaultRowHeight="87.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38.41796875" defaultRowHeight="87.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,10 +494,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -448,54 +506,100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="32.5703125" defaultRowHeight="72.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.578125" defaultRowHeight="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="16384" width="32.5703125" style="1"/>
+    <col min="1" max="1" width="32.578125" style="1"/>
+    <col min="2" max="2" width="79.3125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="32.578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47984206-E65E-41A7-85BC-3EA990641C7B}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="27.1015625" customWidth="1"/>
+    <col min="2" max="2" width="83.62890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="129" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="87.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="97.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[ADD] ajout de fichiers excel de questions
</commit_message>
<xml_diff>
--- a/admin/questions_files/template/Template_Questions.xlsx
+++ b/admin/questions_files/template/Template_Questions.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41630180-EB51-4294-9835-4F43EC660F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="3" r:id="rId1"/>
@@ -13,19 +12,15 @@
     <sheet name="Introduction" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Intitulé de la question (ex : quelle est votre adresse mail ?)</t>
   </si>
   <si>
-    <t>Créer autant de colonnes que de réponses possible (avec leurs noms). Attention si vous avez une réponse autre ne l'ajouté pas en temps que colonne.</t>
-  </si>
-  <si>
     <t>Bouton de validation</t>
   </si>
   <si>
@@ -38,46 +33,28 @@
     <t>Bouton de début de questionnaire</t>
   </si>
   <si>
-    <t>Valider</t>
-  </si>
-  <si>
-    <t>Arrêter le questionnaire</t>
-  </si>
-  <si>
-    <t>Continuer</t>
-  </si>
-  <si>
-    <t>Démarrer</t>
-  </si>
-  <si>
-    <t>Type de réponse attendu : "text", "radio" (choix unique), "checkbox" (choix multiple). Si vous souhaitez indiquer une réponse autre à votre réponse à choix multiple ou unique, indiquer : "checkbox, text" ou "radio, text"</t>
-  </si>
-  <si>
     <t>Combinatoire ( 0 si pas  de réponse particulière est attendu, "2, F" si la réponse attendu à la question de la 2ème ligne est la réponse de la colonne F)</t>
   </si>
   <si>
     <t>RGPD</t>
   </si>
   <si>
-    <t>Ce questionnaire effectue une récolte de vos données personnelles (caractéristiques physiques, goûts, coordonnées notamment) ainsi que de données sur la manière dont vous le remplissez (vitesse, hésitations, changements, etc.). Ces données seront utilisées à des fins de recherches dans le cadre des travaux de Mme Jessica Pidoux. Pour toute demande concernant la gestion des données personnelles, envoyer un mail à l'adresse 'jessica.pidoux@epfl.ch'</t>
-  </si>
-  <si>
     <t>Presentation</t>
   </si>
   <si>
-    <t>Le questionnaire est divisé en plusieurs phases : une phase de questions de départ sur votre sexe et votre orientation sexuelle, plusieurs phases de classement, une phase de questions supplémentaires à la fin. Lors des phases de classement, vous devrez déplacer avec la souris des descriptions de caractéristiques vers une échelle d'importance.</t>
-  </si>
-  <si>
     <t>Validation du RGPD</t>
   </si>
   <si>
-    <t>Cochez la case si vous acceptez les conditions ci-dessus</t>
+    <t>Type de réponse attendu : "text", "radio" (choix unique), "checkbox" (choix multiple). Si vous souhaitez indiquer un champ "Autre" à votre réponse à choix multiple ou unique, indiquer : "checkbox, text" ou "radio, text"</t>
+  </si>
+  <si>
+    <t>Créer autant de colonnes que de réponses possibles (avec leurs noms). Attention si vous avez un champ "Autre" ne l'ajoutez pas en tant que colonne.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,23 +210,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -285,23 +245,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -477,27 +420,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="38.41796875" defaultRowHeight="87.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38.42578125" defaultRowHeight="87.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -506,52 +449,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="32.578125" defaultRowHeight="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.5703125" defaultRowHeight="72.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.578125" style="1"/>
-    <col min="2" max="2" width="79.3125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="32.578125" style="1"/>
+    <col min="1" max="1" width="32.5703125" style="1"/>
+    <col min="2" max="2" width="79.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="32.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -561,42 +492,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47984206-E65E-41A7-85BC-3EA990641C7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1015625" customWidth="1"/>
-    <col min="2" max="2" width="83.62890625" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="83.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="129" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="87.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="97.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>